<commit_message>
first commit from git
</commit_message>
<xml_diff>
--- a/src/test/java/data/userData.xlsx
+++ b/src/test/java/data/userData.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="26925"/>
-  <workbookPr defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{44DF8047-989B-464A-B7FF-8B6C824C41D2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
+  <workbookPr/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191028"/>
+  <calcPr calcId="144525"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -39,28 +38,26 @@
     <t>Mohamed</t>
   </si>
   <si>
-    <t>abdallah@gmail.com</t>
+    <t>klam2@gmail.com</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="2">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="Arial"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
-      <sz val="11"/>
-      <color theme="10"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
+      <sz val="9.8000000000000007"/>
+      <color rgb="FF6AAB73"/>
+      <name val="JetBrains Mono"/>
+      <family val="3"/>
     </font>
   </fonts>
   <fills count="2">
@@ -80,16 +77,16 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="2">
-    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
+  <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -148,7 +145,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin typeface="Calibri Light"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック Light"/>
@@ -200,7 +197,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック"/>
@@ -394,24 +391,24 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col min="2" max="2" width="12.7109375" customWidth="1"/>
-    <col min="3" max="3" width="21.140625" customWidth="1"/>
+    <col min="2" max="2" width="12.75" customWidth="1"/>
+    <col min="3" max="3" width="21.125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4">
@@ -429,9 +426,7 @@
       </c>
     </row>
   </sheetData>
-  <hyperlinks>
-    <hyperlink ref="C1" r:id="rId1" xr:uid="{A556B8D7-478A-4460-A698-57D6419A6C3A}"/>
-  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>